<commit_message>
adds 2022-2024 passage estimates
</commit_message>
<xml_diff>
--- a/data-raw/metadata/battle_upstream_passage_estimates_metadata.xlsx
+++ b/data-raw/metadata/battle_upstream_passage_estimates_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-battle-adult-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-battle-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FA578F-B2BD-CD40-9105-9604E4DC5582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FFD5B6-40BD-7140-A71C-95B064C4747B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="-9480" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59200" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -545,7 +545,7 @@
         <v>1995</v>
       </c>
       <c r="M2" s="6">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>

</xml_diff>